<commit_message>
added v0.2 cutting files
</commit_message>
<xml_diff>
--- a/BOM/lushroom_pi_BOM.xlsx
+++ b/BOM/lushroom_pi_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Arup/Jobs/Lush_Spa/Code/LushRooms/LushRooms/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848F3F33-2B6D-6742-9071-78C6D3DF5861}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA673C1-4D19-2340-A686-8B8362E59F4B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2319,7 +2319,7 @@
   <dimension ref="A1:X998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>